<commit_message>
adjustments for LED library
</commit_message>
<xml_diff>
--- a/data/smiles/template.xlsx
+++ b/data/smiles/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gary/Downloads/zivi/git/delt-core/data/smiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33988A2-4464-1744-8A5E-16EC60F49028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5823F08D-B86E-5D4E-8691-282525AED271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="step1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -87,6 +87,24 @@
   </si>
   <si>
     <t>Complement</t>
+  </si>
+  <si>
+    <t>([#6:1][S;H1:2].[C;H2:3][Cl,Br])&gt;&gt;[#6:1][S:2][C;H2:3]</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>[#6:1][N;H2:2]&gt;&gt;[#6:1][N:2]=[N+]=[N-]</t>
+  </si>
+  <si>
+    <t>[#6:1][S;H1:2].[C;H2:3][Cl,Br]&gt;&gt;[#6:1][S:2][C;H2:3]</t>
+  </si>
+  <si>
+    <t>SN2-2</t>
+  </si>
+  <si>
+    <t>SN2-1</t>
   </si>
 </sst>
 </file>
@@ -365,7 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E613"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10871,7 +10889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AED360-6F4D-9149-A8B6-0C44E6956DF9}">
   <dimension ref="A1:B613"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10935,20 +10953,28 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>

</xml_diff>